<commit_message>
Add cardPuchase and cardStatement
</commit_message>
<xml_diff>
--- a/DotNetExcel/StarkBank.xlsx
+++ b/DotNetExcel/StarkBank.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stark - Admin\Documents\StarkBankExcel - Copia\StarkBankExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6365767D-B608-4419-B612-FA370F10C6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21B3D33-533F-4650-B0FE-F19625A716FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" firstSheet="1" activeTab="1" xr2:uid="{DD233689-9B57-48BF-9576-9FA43391D3F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Principal" sheetId="1" r:id="rId1"/>
-    <sheet name="Credentials" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Credentials" sheetId="2" state="hidden" r:id="rId1"/>
+    <sheet name="Principal" sheetId="1" r:id="rId2"/>
     <sheet name="Compras Cartão" sheetId="12" r:id="rId3"/>
     <sheet name="Extrato Cartão" sheetId="11" r:id="rId4"/>
     <sheet name="Extrato" sheetId="7" r:id="rId5"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
   <si>
     <t>Chave Pix</t>
   </si>
@@ -282,16 +282,10 @@
     <t>Anexo</t>
   </si>
   <si>
-    <t>Descrição Anexo</t>
-  </si>
-  <si>
     <t>ID Cartão</t>
   </si>
   <si>
     <t>ID Holder</t>
-  </si>
-  <si>
-    <t>ID Centro de Custo</t>
   </si>
   <si>
     <t>ID</t>
@@ -301,6 +295,9 @@
   </si>
   <si>
     <t>Cartão Corporativo</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -417,7 +414,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -490,6 +487,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,14 +527,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="28A34ED1D2633F2429D291182761C070389522"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2EF132486228D8243F428A6C298561D10E6622"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -546,14 +544,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1626B229C1652514446181B314A00A77AF6681"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19A5453E610F18142DA1BAA91D29A587ED2E11"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4313"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -563,14 +561,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F70BF05619C7F14D001A2031EA2288CEEF621"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D58F8DCE161321493A19D8C10118F3363B411"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -580,14 +578,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="23FDAD7A329F60245422A56B22EA1482F84402"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="10F831FB013D30140151820D1AB0BB140FD961"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -597,14 +595,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2EF132486228D8243F428A6C298561D10E6622"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="28A34ED1D2633F2429D291182761C070389522"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -614,14 +612,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43935BDA7439194471449D234CFD527D9886B4"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="80815DC5B82C3B8498489E26894C5C52875E28"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1508"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1588"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -631,14 +629,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="71F4FF3617034374D487A4537B51302A0C89B7"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3969"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1720"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -665,14 +663,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="71F4FF3617034374D487A4537B51302A0C89B7"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5FE4E9EDE5117D54C395AB0B52D849B4179075"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3810"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1799"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3836"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1773"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -682,14 +680,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="80815DC5B82C3B8498489E26894C5C52875E28"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43935BDA7439194471449D234CFD527D9886B4"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3784"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3678"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1640"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -699,7 +697,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="75E9B6F4C78CB974E3679B0970BD37E29B8E77"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6D72D142762FA7648186B99160B384DA4EEAD6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -716,19 +714,36 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="10F831FB013D30140151820D1AB0BB140FD961"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="23FDAD7A329F60245422A56B22EA1482F84402"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="576D85FB2525B8547055A14351ED593B73E215"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -745,12 +760,29 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="576D85FB2525B8547055A14351ED593B73E215"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="75E9B6F4C78CB974E3679B0970BD37E29B8E77"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3201"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4BDD5BFBC494C944E75484BA43B9AFC575EDE4"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -762,12 +794,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6D72D142762FA7648186B99160B384DA4EEAD6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -779,7 +811,24 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -796,63 +845,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="21156A5D42671D24110290D22610E26CEF0122"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="36BF4D76D36CAA346A9392633D35C8E7F4F293"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4BDD5BFBC494C944E75484BA43B9AFC575EDE4"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D3C8440119274147F5190E81CB29314F1A0B1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -869,7 +867,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -903,14 +901,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D58F8DCE161321493A19D8C10118F3363B411"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F70BF05619C7F14D001A2031EA2288CEEF621"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -920,7 +918,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4725C0A2E4AB894430D4AEF74EE21D1AD6A734"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F27997732C2CB2441C298BB24A21C18565F42"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -937,7 +935,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5F3C3A5AA5DBB654AFD5A7C25896612CBE6DC5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D3C8440119274147F5190E81CB29314F1A0B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -954,7 +952,24 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6DF62D0586063D64B576813E624CB2DFF23CB6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="190EB7A1C18BFD142EB1A75D1D8ECE9AC6A921"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3096"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -966,7 +981,41 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -983,46 +1032,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4EDC5AE2D4725F442D54BDB348E5FBB86B52C4"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX35.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3443F6D933A917348513994830A35447867593"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX36.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F31A0EA52B80A243F02887A226A80BA2346A2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6DF62D0586063D64B576813E624CB2DFF23CB6"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1034,29 +1049,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX37.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="190EB7A1C18BFD142EB1A75D1D8ECE9AC6A921"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3096"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
 <file path=xl/activeX/activeX38.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="55583C5835971E5409E5944455073F47DDC2A5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="192AED9321906F1430518AA91C61F691A49AE1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1073,7 +1071,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="43443F65340DC5448034B84249A78BF6899C14"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2FAFF23AA2246924D782B58F21CB01DE2B8C82"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1090,14 +1088,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19A5453E610F18142DA1BAA91D29A587ED2E11"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1626B229C1652514446181B314A00A77AF6681"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1124,7 +1122,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2FAFF23AA2246924D782B58F21CB01DE2B8C82"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="43443F65340DC5448034B84249A78BF6899C14"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1141,7 +1139,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="192AED9321906F1430518AA91C61F691A49AE1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="55583C5835971E5409E5944455073F47DDC2A5"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1158,7 +1156,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="5B4A34D975B853543985A7E75523690B60EC35"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1175,7 +1173,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1209,7 +1207,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="207D2713820AB8246622A7CD26A57A9DCA2162"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="42576A9D548EA54490F4BA2045852D9EEA0264"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1226,7 +1224,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="19726D3BD1AD01142191B2C41B5B2D13E650B1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="5B4A34D975B853543985A7E75523690B60EC35"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1243,7 +1241,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="59212E71A5367254941595AB5F075939365595"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1260,7 +1258,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2DE4C20F929D4D245012850329872D57BE1542"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1277,14 +1275,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="17053D61D1F15A1482019B2C1A4E6D57E3A971"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1DB344D2F14249140061BD5D11E614111405C1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4392"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1311,7 +1309,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2DE4C20F929D4D245012850329872D57BE1542"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="482B56B2D4F09144EA9495AD4E1391B3ADA544"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1328,7 +1326,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1441CBD291E7921466418469122C7CFF2CD931"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="59212E71A5367254941595AB5F075939365595"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1345,14 +1343,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="51A95A66553942547D759A7153A00908FCA885"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3281"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1362,7 +1360,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="232EEE2C927B21244D728DA228DC1AAB22C9E2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4E23FE0EC4C93C4470948DA849AEEC73F9C744"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1396,7 +1394,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4E23FE0EC4C93C4470948DA849AEEC73F9C744"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="232EEE2C927B21244D728DA228DC1AAB22C9E2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1413,14 +1411,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="51A95A66553942547D759A7153A00908FCA885"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1B7A977A61ADF41453E1BBBE1183429619DB11"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3281"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1429"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1430,14 +1428,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1F6AA8BD81815014DA61A5D71870FA81614161"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1482"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1447,7 +1445,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1464,14 +1462,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1D1500907189BD14DA51B2181B162FBD75FE31"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1CC3318201EE2A1421C19CEB15987574AED511"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1498,7 +1496,7 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2596667A2285C4241122B3CF25CD7B218043C2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="423CD9C0343555445FB48C9D4CF7D65D1F3284"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -1515,14 +1513,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1F6AA8BD81815014DA61A5D71870FA81614161"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="560AC6FB15F17754F6558A0F58035E0AF7ED85"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1482"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3228"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1535"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1538,8 +1536,8 @@
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1549,14 +1547,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1CC3318201EE2A1421C19CEB15987574AED511"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1D1500907189BD14DA51B2181B162FBD75FE31"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1244"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1376"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1566,14 +1564,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1DB344D2F14249140061BD5D11E614111405C1"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="17053D61D1F15A1482019B2C1A4E6D57E3A971"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3757"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="1217"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="4419"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="1455"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1585,15 +1583,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>361950</xdr:colOff>
+          <xdr:colOff>247649</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>495300</xdr:colOff>
+          <xdr:colOff>581024</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1647,15 +1645,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>161925</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
+          <xdr:colOff>533400</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1709,15 +1707,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>342900</xdr:colOff>
+          <xdr:colOff>266700</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1771,15 +1769,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>180975</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1835,13 +1833,13 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>295275</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>428625</xdr:colOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1895,15 +1893,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>66676</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>438150</xdr:colOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>180976</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1956,16 +1954,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>542925</xdr:colOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>66676</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>180976</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2024,10 +2022,10 @@
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>409575</xdr:colOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2083,13 +2081,13 @@
           <xdr:col>7</xdr:col>
           <xdr:colOff>295275</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>9</xdr:col>
-          <xdr:colOff>428625</xdr:colOff>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2143,15 +2141,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>342900</xdr:colOff>
+          <xdr:colOff>247650</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2205,15 +2203,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>142875</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
+          <xdr:colOff>514350</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2269,13 +2267,13 @@
           <xdr:col>14</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>16</xdr:col>
-          <xdr:colOff>133350</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2331,13 +2329,13 @@
           <xdr:col>13</xdr:col>
           <xdr:colOff>600075</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>16</xdr:col>
-          <xdr:colOff>123825</xdr:colOff>
+          <xdr:colOff>361950</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>123825</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3026,15 +3024,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>990600</xdr:colOff>
+          <xdr:colOff>1019175</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>104775</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>733425</xdr:colOff>
+          <xdr:colOff>714375</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:rowOff>123825</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3088,15 +3086,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>838200</xdr:colOff>
+          <xdr:colOff>857250</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>657225</xdr:colOff>
+          <xdr:colOff>685800</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3150,15 +3148,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>990600</xdr:colOff>
+          <xdr:colOff>1009650</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>733425</xdr:colOff>
+          <xdr:colOff>752475</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3212,15 +3210,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>781050</xdr:colOff>
+          <xdr:colOff>771525</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>161925</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3274,15 +3272,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>838200</xdr:colOff>
+          <xdr:colOff>876300</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>647700</xdr:colOff>
+          <xdr:colOff>676275</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3340,14 +3338,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>314325</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
@@ -3402,14 +3400,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>1200150</xdr:colOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>123825</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>171450</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -3464,14 +3462,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>409575</xdr:colOff>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>476250</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>142875</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -3526,14 +3524,14 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>1190625</xdr:colOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>285750</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>114300</xdr:colOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>161925</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
@@ -5773,12 +5771,670 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F821F73-E4DF-4E63-A6D0-E3043997B034}">
+  <sheetPr codeName="Planilha2"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData/>
+  <dataConsolidate/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3264FF35-57A0-4672-8235-169B3D48197D}">
+  <sheetPr codeName="Planilha10"/>
+  <dimension ref="A1:V9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="20.85546875" style="8" customWidth="1"/>
+    <col min="10" max="19" width="23.85546875" customWidth="1"/>
+    <col min="20" max="22" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="24577" r:id="rId4" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1047750</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="24577" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="24578" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>1285875</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1057275</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="24578" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="24579" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1219200</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="24579" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="24580" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1123950</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>895350</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="24580" r:id="rId10" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="24581" r:id="rId12" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1219200</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>990600</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="24581" r:id="rId12" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF22919-66D6-4ABA-AD2C-41EBDF00D9EF}">
+  <sheetPr codeName="Planilha6"/>
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="19.42578125" style="8" customWidth="1"/>
+    <col min="5" max="9" width="19.42578125" style="16" customWidth="1"/>
+    <col min="10" max="11" width="19.42578125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="33" style="8" customWidth="1"/>
+    <col min="13" max="16" width="19.42578125" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="8197" r:id="rId4" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="8197" r:id="rId4" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="8196" r:id="rId6" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="8196" r:id="rId6" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="8195" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1276350</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="8195" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="8194" r:id="rId10" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1247775</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="8194" r:id="rId10" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="8193" r:id="rId12" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1257300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="8193" r:id="rId12" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04BC81C-AF4F-4056-AB23-1893055E9200}">
+  <sheetPr codeName="Planilha5"/>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="16" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="8" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="16" customWidth="1"/>
+    <col min="7" max="13" width="20.7109375" style="8" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A9:M9" xr:uid="{D04BC81C-AF4F-4056-AB23-1893055E9200}"/>
+  <dataConsolidate/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>123825</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1266825</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>123825</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1285875</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6147" r:id="rId8" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1228725</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6147" r:id="rId8" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6148" r:id="rId10" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1362075</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6148" r:id="rId10" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6149" r:id="rId12" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1228725</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6149" r:id="rId12" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9CDEB5-694E-4A1B-9CEB-80FED39AC6B0}">
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -5788,28 +6444,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -6000,32 +6656,32 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
@@ -6094,30 +6750,30 @@
       <c r="T13" s="17"/>
     </row>
     <row r="14" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="27"/>
-      <c r="T14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
@@ -6186,30 +6842,30 @@
       <c r="T17" s="17"/>
     </row>
     <row r="18" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="17"/>
@@ -6298,19 +6954,69 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1044" r:id="rId4" name="_ActiveXWrapper11">
+        <control shapeId="1046" r:id="rId4" name="_ActiveXWrapper13">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>361950</xdr:colOff>
                 <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1046" r:id="rId4" name="_ActiveXWrapper13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1045" r:id="rId6" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>14</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>16</xdr:col>
+                <xdr:colOff>371475</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1045" r:id="rId6" name="_ActiveXWrapper12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId8" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
@@ -6318,132 +7024,82 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1044" r:id="rId4" name="_ActiveXWrapper11"/>
+        <control shapeId="1041" r:id="rId8" name="_ActiveXWrapper8"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1043" r:id="rId6" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1040" r:id="rId10" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>342900</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1043" r:id="rId6" name="_ActiveXWrapper10"/>
+        <control shapeId="1040" r:id="rId10" name="_ActiveXWrapper7"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId8" name="_ActiveXWrapper9">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="1039" r:id="rId12" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1042" r:id="rId8" name="_ActiveXWrapper9"/>
+        <control shapeId="1039" r:id="rId12" name="_ActiveXWrapper6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
+        <control shapeId="1038" r:id="rId14" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>361950</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>495300</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId10" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId12" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId12" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>342900</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper3"/>
+        <control shapeId="1038" r:id="rId14" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6453,15 +7109,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
+                <xdr:colOff>180975</xdr:colOff>
                 <xdr:row>18</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>1048575</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -6473,342 +7129,44 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId18" name="_ActiveXWrapper5">
+        <control shapeId="1036" r:id="rId18" name="_ActiveXWrapper3">
           <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>266700</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>1048575</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1038" r:id="rId18" name="_ActiveXWrapper5"/>
+        <control shapeId="1036" r:id="rId18" name="_ActiveXWrapper3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId20" name="_ActiveXWrapper6">
+        <control shapeId="1035" r:id="rId20" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId21">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>304800</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>438150</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1039" r:id="rId20" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId22" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>542925</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1040" r:id="rId22" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId24" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>409575</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1041" r:id="rId24" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1045" r:id="rId26" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>14</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>133350</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
                 <xdr:row>12</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1045" r:id="rId26" name="_ActiveXWrapper12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId28" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>16</xdr:col>
-                <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>16</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1046" r:id="rId28" name="_ActiveXWrapper13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </controls>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3264FF35-57A0-4672-8235-169B3D48197D}">
-  <sheetPr codeName="Planilha10"/>
-  <dimension ref="A1:V9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="9" width="20.85546875" style="8" customWidth="1"/>
-    <col min="10" max="19" width="23.85546875" customWidth="1"/>
-    <col min="20" max="22" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <controls>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="24581" r:id="rId4" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1219200</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="24581" r:id="rId4" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="24580" r:id="rId6" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1123950</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>895350</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="24580" r:id="rId6" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="24579" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1219200</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="24579" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="24578" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1285875</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1057275</xdr:colOff>
-                <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
@@ -6816,471 +7174,110 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24578" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="1035" r:id="rId20" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="24577" r:id="rId12" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="1025" r:id="rId22" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>1047750</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="24577" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="1025" r:id="rId22" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
-  </controls>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF22919-66D6-4ABA-AD2C-41EBDF00D9EF}">
-  <sheetPr codeName="Planilha6"/>
-  <dimension ref="A1:P9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="19.42578125" style="8" customWidth="1"/>
-    <col min="5" max="9" width="19.42578125" style="16" customWidth="1"/>
-    <col min="10" max="11" width="19.42578125" style="8" customWidth="1"/>
-    <col min="12" max="12" width="33" style="8" customWidth="1"/>
-    <col min="13" max="16" width="19.42578125" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8193" r:id="rId4" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="1042" r:id="rId24" name="_ActiveXWrapper9">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1257300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>161925</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8193" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="1042" r:id="rId24" name="_ActiveXWrapper9"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8194" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1043" r:id="rId26" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId27">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>247650</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1247775</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8194" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="1043" r:id="rId26" name="_ActiveXWrapper10"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="8195" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="1044" r:id="rId28" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId29">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>514350</xdr:colOff>
+                <xdr:row>16</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="8195" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="8196" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="8196" r:id="rId10" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="8197" r:id="rId12" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1276350</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="8197" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="1044" r:id="rId28" name="_ActiveXWrapper11"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04BC81C-AF4F-4056-AB23-1893055E9200}">
-  <sheetPr codeName="Planilha5"/>
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="20.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="8" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="16" customWidth="1"/>
-    <col min="7" max="13" width="20.7109375" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" hidden="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A9:M9" xr:uid="{D04BC81C-AF4F-4056-AB23-1893055E9200}"/>
-  <dataConsolidate/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <controls>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6149" r:id="rId4" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1228725</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6149" r:id="rId4" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6148" r:id="rId6" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1362075</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1143000</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6148" r:id="rId6" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6147" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1228725</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6147" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6146" r:id="rId10" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1285875</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6146" r:id="rId10" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6145" r:id="rId12" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1266825</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6145" r:id="rId12" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </controls>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F821F73-E4DF-4E63-A6D0-E3043997B034}">
-  <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="8"/>
-  </cols>
-  <sheetData/>
-  <dataConsolidate/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7289,8 +7286,8 @@
   <sheetPr codeName="Planilha12"/>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7305,12 +7302,12 @@
     <col min="8" max="8" width="18.7109375" style="8" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="17"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -7321,10 +7318,8 @@
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -7335,10 +7330,8 @@
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -7349,10 +7342,8 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -7363,10 +7354,8 @@
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -7377,10 +7366,8 @@
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -7391,10 +7378,8 @@
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -7405,10 +7390,8 @@
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -7419,10 +7402,8 @@
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>44</v>
       </c>
@@ -7452,12 +7433,6 @@
       </c>
       <c r="J9" s="20" t="s">
         <v>76</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -7469,52 +7444,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37892" r:id="rId4" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="37896" r:id="rId4" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>876300</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>733425</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>114300</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37892" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="37896" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37893" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="37895" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>657225</xdr:colOff>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37893" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="37895" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -7524,15 +7499,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>990600</xdr:colOff>
+                <xdr:colOff>1009650</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>733425</xdr:colOff>
+                <xdr:colOff>752475</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -7544,52 +7519,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37895" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="37893" r:id="rId10" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>781050</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>685800</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37895" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="37893" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="37896" r:id="rId12" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="37892" r:id="rId12" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1019175</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:rowOff>104775</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>714375</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>123825</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="37896" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="37892" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7601,8 +7576,8 @@
   <sheetPr codeName="Planilha11"/>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7610,10 +7585,10 @@
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="20" style="27" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="10" width="9.140625" style="8" hidden="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" hidden="1"/>
@@ -7719,7 +7694,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>70</v>
@@ -7731,13 +7706,13 @@
         <v>1</v>
       </c>
       <c r="F9" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>1</v>
-      </c>
       <c r="H9" s="20" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7749,18 +7724,93 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="28679" r:id="rId4" name="_ActiveXWrapper11">
+        <control shapeId="28678" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1190625</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28678" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28677" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28677" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28676" r:id="rId8" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>314325</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>142875</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="28676" r:id="rId8" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="28679" r:id="rId10" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
                 <xdr:row>7</xdr:row>
                 <xdr:rowOff>104775</xdr:rowOff>
               </to>
@@ -7769,82 +7819,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="28679" r:id="rId4" name="_ActiveXWrapper11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28676" r:id="rId6" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>333375</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28676" r:id="rId6" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28677" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>123825</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28677" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="28678" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>409575</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="28678" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="28679" r:id="rId10" name="_ActiveXWrapper11"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7857,7 +7832,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:I9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7917,8 +7892,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="10241" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="10244" r:id="rId4" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1371600</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1143000</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10244" r:id="rId4" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10243" r:id="rId6" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1247775</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10243" r:id="rId6" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10242" r:id="rId8" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>171450</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1333500</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="10242" r:id="rId8" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="10241" r:id="rId10" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
@@ -7937,82 +7987,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="10241" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10242" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1333500</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10242" r:id="rId6" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10243" r:id="rId8" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1247775</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10243" r:id="rId8" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="10244" r:id="rId10" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1371600</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1143000</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="10244" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="10241" r:id="rId10" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8024,7 +7999,7 @@
   <sheetPr codeName="Planilha4"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -8083,52 +8058,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4097" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="4101" r:id="rId4" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1381125</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1228725</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>1152525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4097" r:id="rId4" name="_ActiveXWrapper1"/>
+        <control shapeId="4101" r:id="rId4" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4098" r:id="rId6" name="_ActiveXWrapper2">
+        <control shapeId="4100" r:id="rId6" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4098" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="4100" r:id="rId6" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8158,52 +8133,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4100" r:id="rId10" name="_ActiveXWrapper4">
+        <control shapeId="4098" r:id="rId10" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>1200150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4100" r:id="rId10" name="_ActiveXWrapper4"/>
+        <control shapeId="4098" r:id="rId10" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="4101" r:id="rId12" name="_ActiveXWrapper5">
+        <control shapeId="4097" r:id="rId12" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1381125</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>1152525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1228725</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="4101" r:id="rId12" name="_ActiveXWrapper5"/>
+        <control shapeId="4097" r:id="rId12" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8215,7 +8190,7 @@
   <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -8283,8 +8258,133 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3078" r:id="rId4" name="_ActiveXWrapper6">
+        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>542925</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3073" r:id="rId4" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3074" r:id="rId6" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>295275</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3074" r:id="rId6" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3075" r:id="rId8" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3075" r:id="rId8" name="_ActiveXWrapper7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3076" r:id="rId10" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>723900</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3076" r:id="rId10" name="_ActiveXWrapper8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3077" r:id="rId12" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>581025</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>276225</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3077" r:id="rId12" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3078" r:id="rId14" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
@@ -8303,132 +8403,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3078" r:id="rId4" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3077" r:id="rId6" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>276225</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3077" r:id="rId6" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3076" r:id="rId8" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>723900</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3076" r:id="rId8" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3075" r:id="rId10" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>581025</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3075" r:id="rId10" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3074" r:id="rId12" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>295275</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3074" r:id="rId12" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3073" r:id="rId14" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>542925</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3073" r:id="rId14" name="_ActiveXWrapper1"/>
+        <control shapeId="3078" r:id="rId14" name="_ActiveXWrapper6"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8441,7 +8416,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8544,18 +8519,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="16389" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="16385" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>1323975</xdr:colOff>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1095375</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1162050</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -8564,23 +8539,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="16389" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="16385" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="16388" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="16386" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1200150</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>971550</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>1162050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>57150</xdr:rowOff>
               </to>
@@ -8589,7 +8564,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="16388" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="16386" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8619,18 +8594,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="16386" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="16388" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1200150</xdr:colOff>
                 <xdr:row>0</xdr:row>
                 <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1162050</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>971550</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>57150</xdr:rowOff>
               </to>
@@ -8639,23 +8614,23 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="16386" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="16388" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="16385" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="16389" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>1323975</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>1162050</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1095375</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -8664,7 +8639,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="16385" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="16389" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8778,52 +8753,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20485" r:id="rId4" name="_ActiveXWrapper5">
+        <control shapeId="20481" r:id="rId4" name="_ActiveXWrapper1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>257175</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>38100</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20485" r:id="rId4" name="_ActiveXWrapper5"/>
+        <control shapeId="20481" r:id="rId4" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20484" r:id="rId6" name="_ActiveXWrapper4">
+        <control shapeId="20482" r:id="rId6" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>390525</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:rowOff>161925</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20484" r:id="rId6" name="_ActiveXWrapper4"/>
+        <control shapeId="20482" r:id="rId6" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8853,52 +8828,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20482" r:id="rId10" name="_ActiveXWrapper2">
+        <control shapeId="20484" r:id="rId10" name="_ActiveXWrapper4">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>390525</xdr:colOff>
                 <xdr:row>0</xdr:row>
-                <xdr:rowOff>161925</xdr:rowOff>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>219075</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20482" r:id="rId10" name="_ActiveXWrapper2"/>
+        <control shapeId="20484" r:id="rId10" name="_ActiveXWrapper4"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="20481" r:id="rId12" name="_ActiveXWrapper1">
+        <control shapeId="20485" r:id="rId12" name="_ActiveXWrapper5">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>238125</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>76200</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="20481" r:id="rId12" name="_ActiveXWrapper1"/>
+        <control shapeId="20485" r:id="rId12" name="_ActiveXWrapper5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>